<commit_message>
Fixed 'prop urban in Co-located modes data file
</commit_message>
<xml_diff>
--- a/Cluster analysis results/Final Cluster solution/Mean diff calculations.xlsx
+++ b/Cluster analysis results/Final Cluster solution/Mean diff calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lkast1\Google Drive\PhD\2.Analysis\2. Empirical Analysis\BE-TR_Multi Country Samples\Melbourne\Melb.All.Stops\Melb.AllStops.Repo\Cluster analysis results\Final Cluster solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED4684D-E68E-44EB-A985-B43B04443989}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3472D2-792B-47B9-A491-3DF04A5EEED3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250" xr2:uid="{41582402-FDA3-4143-9721-5883E471C988}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
   <si>
     <t>d</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Average of_PBN</t>
+  </si>
+  <si>
+    <t>SUM</t>
   </si>
 </sst>
 </file>
@@ -204,7 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -228,6 +231,9 @@
     <xf numFmtId="4" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -595,13 +601,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7B07C3-6AF8-46FA-A6E8-72F64D635A3A}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="C1:Y29"/>
+  <dimension ref="C1:Z29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U22" sqref="U22:W24"/>
+      <selection pane="bottomRight" activeCell="M1" sqref="M1:W1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -613,31 +619,34 @@
     <col min="11" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.36328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.26953125" customWidth="1"/>
-    <col min="15" max="15" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.26953125" customWidth="1"/>
+    <col min="16" max="16" width="11.08984375" customWidth="1"/>
+    <col min="17" max="18" width="12.1796875" customWidth="1"/>
+    <col min="19" max="20" width="8.7265625" customWidth="1"/>
+    <col min="21" max="21" width="12" customWidth="1"/>
+    <col min="22" max="23" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:25" x14ac:dyDescent="0.35">
-      <c r="D1" s="12" t="s">
+    <row r="1" spans="3:26" x14ac:dyDescent="0.35">
+      <c r="D1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-    </row>
-    <row r="2" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+    </row>
+    <row r="2" spans="3:26" x14ac:dyDescent="0.35">
       <c r="D2" t="s">
         <v>2</v>
       </c>
@@ -668,35 +677,35 @@
       <c r="N2" t="s">
         <v>27</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>2</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>3</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>25</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>26</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>27</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>25</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>26</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="3:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>1</v>
       </c>
@@ -733,8 +742,8 @@
       <c r="N3" t="s">
         <v>29</v>
       </c>
-      <c r="R3" t="s">
-        <v>0</v>
+      <c r="O3" t="s">
+        <v>37</v>
       </c>
       <c r="S3" t="s">
         <v>0</v>
@@ -743,7 +752,7 @@
         <v>0</v>
       </c>
       <c r="U3" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="V3" t="s">
         <v>29</v>
@@ -751,8 +760,14 @@
       <c r="W3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="X3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>6</v>
       </c>
@@ -772,15 +787,15 @@
         <v>1.419237917973851</v>
       </c>
       <c r="I4" s="2">
-        <f>E4-D4</f>
+        <f t="shared" ref="I4:I20" si="0">E4-D4</f>
         <v>1.891144503646867</v>
       </c>
       <c r="J4" s="2">
-        <f>F4-D4</f>
+        <f t="shared" ref="J4:J20" si="1">F4-D4</f>
         <v>0.73952152845795371</v>
       </c>
       <c r="K4" s="2">
-        <f>F4-E4</f>
+        <f t="shared" ref="K4:K20" si="2">F4-E4</f>
         <v>-1.1516229751889133</v>
       </c>
       <c r="L4" s="2">
@@ -788,50 +803,57 @@
         <v>1.3325070304961446</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" ref="M4:N4" si="0">ABS(J4)/$H4</f>
+        <f t="shared" ref="M4:N4" si="3">ABS(J4)/$H4</f>
         <v>0.5210694550168995</v>
       </c>
       <c r="N4" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.811437575479245</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="10">
+        <f>SUM(L4:N4)</f>
+        <v>2.6650140609922892</v>
+      </c>
+      <c r="P4" s="2">
         <v>6.7867747390108715</v>
       </c>
-      <c r="P4" s="2">
+      <c r="Q4" s="2">
         <v>7.3499336093276293</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="R4" s="2">
         <v>6.7529455258384026</v>
       </c>
-      <c r="R4" s="2">
-        <f>P4-O4</f>
+      <c r="S4" s="2">
+        <f>Q4-P4</f>
         <v>0.56315887031675782</v>
       </c>
-      <c r="S4" s="2">
-        <f>Q4-O4</f>
+      <c r="T4" s="2">
+        <f>R4-P4</f>
         <v>-3.3829213172468897E-2</v>
       </c>
-      <c r="T4" s="2">
-        <f>Q4-P4</f>
+      <c r="U4" s="2">
+        <f>R4-Q4</f>
         <v>-0.59698808348922672</v>
       </c>
-      <c r="U4" s="2">
-        <f>ABS(R4)/$H4</f>
+      <c r="V4" s="2">
+        <f>ABS(S4)/$H4</f>
         <v>0.39680370936026094</v>
       </c>
-      <c r="V4" s="2">
-        <f t="shared" ref="V4" si="1">ABS(S4)/$H4</f>
+      <c r="W4" s="2">
+        <f t="shared" ref="W4" si="4">ABS(T4)/$H4</f>
         <v>2.3836181900188061E-2</v>
       </c>
-      <c r="W4" s="2">
-        <f t="shared" ref="W4" si="2">ABS(T4)/$H4</f>
+      <c r="X4" s="2">
+        <f t="shared" ref="X4" si="5">ABS(U4)/$H4</f>
         <v>0.42063989126044898</v>
       </c>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-    </row>
-    <row r="5" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y4" s="2">
+        <f>SUM(V4:X4)</f>
+        <v>0.84127978252089797</v>
+      </c>
+      <c r="Z4" s="2"/>
+    </row>
+    <row r="5" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>7</v>
       </c>
@@ -851,66 +873,73 @@
         <v>1.0531815777144569</v>
       </c>
       <c r="I5" s="2">
-        <f>E5-D5</f>
+        <f t="shared" si="0"/>
         <v>0.85224378664911349</v>
       </c>
       <c r="J5" s="2">
-        <f>F5-D5</f>
+        <f t="shared" si="1"/>
         <v>0.31041930367242809</v>
       </c>
       <c r="K5" s="2">
-        <f>F5-E5</f>
+        <f t="shared" si="2"/>
         <v>-0.5418244829766854</v>
       </c>
       <c r="L5" s="2">
-        <f t="shared" ref="L5:L20" si="3">ABS(I5)/$H5</f>
+        <f t="shared" ref="L5:L20" si="6">ABS(I5)/$H5</f>
         <v>0.80920878667341967</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" ref="M5:M20" si="4">ABS(J5)/$H5</f>
+        <f t="shared" ref="M5:M20" si="7">ABS(J5)/$H5</f>
         <v>0.29474433491903551</v>
       </c>
       <c r="N5" s="2">
-        <f t="shared" ref="N5:N20" si="5">ABS(K5)/$H5</f>
+        <f t="shared" ref="N5:N20" si="8">ABS(K5)/$H5</f>
         <v>0.51446445175438416</v>
       </c>
       <c r="O5" s="2">
+        <f t="shared" ref="O5:O25" si="9">SUM(L5:N5)</f>
+        <v>1.6184175733468393</v>
+      </c>
+      <c r="P5" s="2">
         <v>8.0365053785740201</v>
       </c>
-      <c r="P5" s="2">
+      <c r="Q5" s="2">
         <v>8.1522672233340145</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="R5" s="2">
         <v>7.8550043743657314</v>
       </c>
-      <c r="R5" s="2">
-        <f t="shared" ref="R5:R20" si="6">P5-O5</f>
+      <c r="S5" s="2">
+        <f t="shared" ref="S5:S20" si="10">Q5-P5</f>
         <v>0.1157618447599944</v>
       </c>
-      <c r="S5" s="2">
-        <f t="shared" ref="S5:S20" si="7">Q5-O5</f>
+      <c r="T5" s="2">
+        <f t="shared" ref="T5:T20" si="11">R5-P5</f>
         <v>-0.18150100420828874</v>
       </c>
-      <c r="T5" s="2">
-        <f t="shared" ref="T5:T20" si="8">Q5-P5</f>
+      <c r="U5" s="2">
+        <f t="shared" ref="U5:U20" si="12">R5-Q5</f>
         <v>-0.29726284896828314</v>
       </c>
-      <c r="U5" s="2">
-        <f t="shared" ref="U5:U20" si="9">ABS(R5)/$H5</f>
+      <c r="V5" s="2">
+        <f t="shared" ref="V5:V20" si="13">ABS(S5)/$H5</f>
         <v>0.10991632137281863</v>
       </c>
-      <c r="V5" s="2">
-        <f t="shared" ref="V5:V20" si="10">ABS(S5)/$H5</f>
+      <c r="W5" s="2">
+        <f t="shared" ref="W5:W20" si="14">ABS(T5)/$H5</f>
         <v>0.17233590868743631</v>
       </c>
-      <c r="W5" s="2">
-        <f t="shared" ref="W5:W20" si="11">ABS(T5)/$H5</f>
+      <c r="X5" s="2">
+        <f t="shared" ref="X5:X20" si="15">ABS(U5)/$H5</f>
         <v>0.28225223006025496</v>
       </c>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-    </row>
-    <row r="6" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y5" s="2">
+        <f t="shared" ref="Y5:Y24" si="16">SUM(V5:X5)</f>
+        <v>0.56450446012050992</v>
+      </c>
+      <c r="Z5" s="2"/>
+    </row>
+    <row r="6" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>8</v>
       </c>
@@ -930,66 +959,73 @@
         <v>0.18362625194115237</v>
       </c>
       <c r="I6" s="5">
-        <f>E6-D6</f>
+        <f t="shared" si="0"/>
         <v>0.11292931484567319</v>
       </c>
       <c r="J6" s="5">
-        <f>F6-D6</f>
+        <f t="shared" si="1"/>
         <v>6.4178853294616658E-2</v>
       </c>
       <c r="K6" s="5">
-        <f>F6-E6</f>
+        <f t="shared" si="2"/>
         <v>-4.8750461551056529E-2</v>
       </c>
       <c r="L6" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.61499547941469834</v>
       </c>
       <c r="M6" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.34950805027150683</v>
       </c>
       <c r="N6" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.26548742914319157</v>
       </c>
       <c r="O6" s="2">
+        <f t="shared" si="9"/>
+        <v>1.2299909588293967</v>
+      </c>
+      <c r="P6" s="2">
         <v>0.1337552085896227</v>
       </c>
-      <c r="P6" s="2">
+      <c r="Q6" s="2">
         <v>0.14075565980188681</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="R6" s="2">
         <v>0.14556432970754712</v>
       </c>
-      <c r="R6" s="5">
-        <f t="shared" si="6"/>
+      <c r="S6" s="5">
+        <f t="shared" si="10"/>
         <v>7.0004512122641138E-3</v>
       </c>
-      <c r="S6" s="5">
-        <f t="shared" si="7"/>
+      <c r="T6" s="5">
+        <f t="shared" si="11"/>
         <v>1.1809121117924426E-2</v>
       </c>
-      <c r="T6" s="5">
-        <f t="shared" si="8"/>
+      <c r="U6" s="5">
+        <f t="shared" si="12"/>
         <v>4.8086699056603122E-3</v>
       </c>
-      <c r="U6" s="2">
-        <f t="shared" si="9"/>
+      <c r="V6" s="2">
+        <f t="shared" si="13"/>
         <v>3.8123368190881461E-2</v>
       </c>
-      <c r="V6" s="2">
-        <f t="shared" si="10"/>
+      <c r="W6" s="2">
+        <f t="shared" si="14"/>
         <v>6.4310636377357164E-2</v>
       </c>
-      <c r="W6" s="2">
-        <f t="shared" si="11"/>
+      <c r="X6" s="2">
+        <f t="shared" si="15"/>
         <v>2.6187268186475706E-2</v>
       </c>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-    </row>
-    <row r="7" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y6" s="2">
+        <f t="shared" si="16"/>
+        <v>0.12862127275471433</v>
+      </c>
+      <c r="Z6" s="2"/>
+    </row>
+    <row r="7" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>9</v>
       </c>
@@ -1009,66 +1045,73 @@
         <v>0.12227649776527212</v>
       </c>
       <c r="I7" s="2">
-        <f>E7-D7</f>
+        <f t="shared" si="0"/>
         <v>6.3843037126867994E-2</v>
       </c>
       <c r="J7" s="2">
-        <f>F7-D7</f>
+        <f t="shared" si="1"/>
         <v>1.5940409016818827E-2</v>
       </c>
       <c r="K7" s="2">
-        <f>F7-E7</f>
+        <f t="shared" si="2"/>
         <v>-4.7902628110049167E-2</v>
       </c>
       <c r="L7" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.52212026263153344</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.13036363739676946</v>
       </c>
       <c r="N7" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.39175662523476401</v>
       </c>
       <c r="O7" s="2">
+        <f t="shared" si="9"/>
+        <v>1.0442405252630669</v>
+      </c>
+      <c r="P7" s="2">
         <v>8.7026740589622689E-2</v>
       </c>
-      <c r="P7" s="2">
+      <c r="Q7" s="2">
         <v>0.11597195491509435</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="R7" s="2">
         <v>9.4714809632075417E-2</v>
       </c>
-      <c r="R7" s="2">
-        <f t="shared" si="6"/>
+      <c r="S7" s="2">
+        <f t="shared" si="10"/>
         <v>2.894521432547166E-2</v>
       </c>
-      <c r="S7" s="2">
-        <f t="shared" si="7"/>
+      <c r="T7" s="2">
+        <f t="shared" si="11"/>
         <v>7.6880690424527276E-3</v>
       </c>
-      <c r="T7" s="2">
-        <f t="shared" si="8"/>
+      <c r="U7" s="2">
+        <f t="shared" si="12"/>
         <v>-2.1257145283018933E-2</v>
       </c>
-      <c r="U7" s="2">
-        <f t="shared" si="9"/>
+      <c r="V7" s="2">
+        <f t="shared" si="13"/>
         <v>0.2367193602570814</v>
       </c>
-      <c r="V7" s="2">
-        <f t="shared" si="10"/>
+      <c r="W7" s="2">
+        <f t="shared" si="14"/>
         <v>6.2874462247120594E-2</v>
       </c>
-      <c r="W7" s="2">
-        <f t="shared" si="11"/>
+      <c r="X7" s="2">
+        <f t="shared" si="15"/>
         <v>0.17384489800996081</v>
       </c>
-      <c r="X7" s="10"/>
-      <c r="Y7" s="2"/>
-    </row>
-    <row r="8" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y7" s="2">
+        <f t="shared" si="16"/>
+        <v>0.4734387205141628</v>
+      </c>
+      <c r="Z7" s="2"/>
+    </row>
+    <row r="8" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>11</v>
       </c>
@@ -1088,66 +1131,73 @@
         <v>37.34177591272973</v>
       </c>
       <c r="I8" s="2">
-        <f>E8-D8</f>
+        <f t="shared" si="0"/>
         <v>33.580428167168719</v>
       </c>
       <c r="J8" s="2">
-        <f>F8-D8</f>
+        <f t="shared" si="1"/>
         <v>8.4415410026052768</v>
       </c>
       <c r="K8" s="2">
-        <f>F8-E8</f>
+        <f t="shared" si="2"/>
         <v>-25.138887164563442</v>
       </c>
       <c r="L8" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.89927239255166824</v>
       </c>
       <c r="M8" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.22606158374292995</v>
       </c>
       <c r="N8" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.67321080880873829</v>
       </c>
       <c r="O8" s="2">
+        <f t="shared" si="9"/>
+        <v>1.7985447851033365</v>
+      </c>
+      <c r="P8" s="2">
         <v>101.6787553961563</v>
       </c>
-      <c r="P8" s="2">
+      <c r="Q8" s="2">
         <v>96.546185939056969</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="R8" s="2">
         <v>89.956403814968255</v>
       </c>
-      <c r="R8" s="2">
-        <f t="shared" si="6"/>
+      <c r="S8" s="2">
+        <f t="shared" si="10"/>
         <v>-5.1325694570993363</v>
       </c>
-      <c r="S8" s="2">
-        <f t="shared" si="7"/>
+      <c r="T8" s="2">
+        <f t="shared" si="11"/>
         <v>-11.72235158118805</v>
       </c>
-      <c r="T8" s="2">
-        <f t="shared" si="8"/>
+      <c r="U8" s="2">
+        <f t="shared" si="12"/>
         <v>-6.589782124088714</v>
       </c>
-      <c r="U8" s="2">
-        <f t="shared" si="9"/>
+      <c r="V8" s="2">
+        <f t="shared" si="13"/>
         <v>0.13744845636411349</v>
       </c>
-      <c r="V8" s="2">
-        <f t="shared" si="10"/>
+      <c r="W8" s="2">
+        <f t="shared" si="14"/>
         <v>0.3139205700495869</v>
       </c>
-      <c r="W8" s="2">
-        <f t="shared" si="11"/>
+      <c r="X8" s="2">
+        <f t="shared" si="15"/>
         <v>0.17647211368547341</v>
       </c>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-    </row>
-    <row r="9" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y8" s="2">
+        <f t="shared" si="16"/>
+        <v>0.6278411400991738</v>
+      </c>
+      <c r="Z8" s="2"/>
+    </row>
+    <row r="9" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>36</v>
       </c>
@@ -1167,66 +1217,73 @@
         <v>0.16174767030556705</v>
       </c>
       <c r="I9" s="2">
-        <f>E9-D9</f>
+        <f t="shared" si="0"/>
         <v>0.12523970896887995</v>
       </c>
       <c r="J9" s="2">
-        <f>F9-D9</f>
+        <f t="shared" si="1"/>
         <v>6.7524377544285363E-2</v>
       </c>
       <c r="K9" s="2">
-        <f>F9-E9</f>
+        <f t="shared" si="2"/>
         <v>-5.771533142459459E-2</v>
       </c>
       <c r="L9" s="2">
-        <f t="shared" ref="L9" si="12">ABS(I9)/$H9</f>
+        <f t="shared" ref="L9" si="17">ABS(I9)/$H9</f>
         <v>0.7742906511870139</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" ref="M9" si="13">ABS(J9)/$H9</f>
+        <f t="shared" ref="M9" si="18">ABS(J9)/$H9</f>
         <v>0.41746738865988664</v>
       </c>
       <c r="N9" s="2">
-        <f t="shared" ref="N9" si="14">ABS(K9)/$H9</f>
+        <f t="shared" ref="N9" si="19">ABS(K9)/$H9</f>
         <v>0.35682326252712732</v>
       </c>
-      <c r="O9" s="13">
+      <c r="O9" s="2">
+        <f t="shared" si="9"/>
+        <v>1.5485813023740278</v>
+      </c>
+      <c r="P9" s="13">
         <v>0.11362281454716983</v>
       </c>
-      <c r="P9" s="13">
+      <c r="Q9" s="13">
         <v>0.16122358821226412</v>
       </c>
-      <c r="Q9" s="13">
+      <c r="R9" s="13">
         <v>0.15252172070754727</v>
       </c>
-      <c r="R9" s="2">
-        <f t="shared" ref="R9" si="15">P9-O9</f>
+      <c r="S9" s="2">
+        <f t="shared" ref="S9" si="20">Q9-P9</f>
         <v>4.7600773665094298E-2</v>
       </c>
-      <c r="S9" s="2">
-        <f t="shared" ref="S9" si="16">Q9-O9</f>
+      <c r="T9" s="2">
+        <f t="shared" ref="T9" si="21">R9-P9</f>
         <v>3.8898906160377444E-2</v>
       </c>
-      <c r="T9" s="2">
-        <f t="shared" ref="T9" si="17">Q9-P9</f>
+      <c r="U9" s="2">
+        <f t="shared" ref="U9" si="22">R9-Q9</f>
         <v>-8.7018675047168537E-3</v>
       </c>
-      <c r="U9" s="2">
-        <f t="shared" ref="U9" si="18">ABS(R9)/$H9</f>
+      <c r="V9" s="2">
+        <f t="shared" ref="V9" si="23">ABS(S9)/$H9</f>
         <v>0.29429032007180611</v>
       </c>
-      <c r="V9" s="2">
-        <f t="shared" ref="V9" si="19">ABS(S9)/$H9</f>
+      <c r="W9" s="2">
+        <f t="shared" ref="W9" si="24">ABS(T9)/$H9</f>
         <v>0.24049129169459585</v>
       </c>
-      <c r="W9" s="2">
-        <f t="shared" ref="W9" si="20">ABS(T9)/$H9</f>
+      <c r="X9" s="2">
+        <f t="shared" ref="X9" si="25">ABS(U9)/$H9</f>
         <v>5.3799028377210276E-2</v>
       </c>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
-    </row>
-    <row r="10" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y9" s="2">
+        <f t="shared" si="16"/>
+        <v>0.58858064014361222</v>
+      </c>
+      <c r="Z9" s="2"/>
+    </row>
+    <row r="10" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>14</v>
       </c>
@@ -1246,15 +1303,15 @@
         <v>2.6154537934430295</v>
       </c>
       <c r="I10" s="2">
-        <f>E10-D10</f>
+        <f t="shared" si="0"/>
         <v>-1.274043542975144</v>
       </c>
       <c r="J10" s="2">
-        <f>F10-D10</f>
+        <f t="shared" si="1"/>
         <v>-0.96514140538472848</v>
       </c>
       <c r="K10" s="2">
-        <f>F10-E10</f>
+        <f t="shared" si="2"/>
         <v>0.30890213759041552</v>
       </c>
       <c r="L10" s="2">
@@ -1270,42 +1327,49 @@
         <v>0.11810651687475285</v>
       </c>
       <c r="O10" s="2">
+        <f t="shared" si="9"/>
+        <v>0.97424282254130024</v>
+      </c>
+      <c r="P10" s="2">
         <v>1.5282349640283031</v>
       </c>
-      <c r="P10" s="2">
+      <c r="Q10" s="2">
         <v>1.3551512534386791</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="R10" s="2">
         <v>1.3661916780424532</v>
       </c>
-      <c r="R10" s="2">
-        <f>P10-O10</f>
+      <c r="S10" s="2">
+        <f>Q10-P10</f>
         <v>-0.17308371058962391</v>
       </c>
-      <c r="S10" s="2">
-        <f>Q10-O10</f>
+      <c r="T10" s="2">
+        <f>R10-P10</f>
         <v>-0.16204328598584983</v>
       </c>
-      <c r="T10" s="2">
-        <f>Q10-P10</f>
+      <c r="U10" s="2">
+        <f>R10-Q10</f>
         <v>1.1040424603774079E-2</v>
-      </c>
-      <c r="U10" s="2">
-        <f>ABS(R10)/$H10</f>
-        <v>6.6177315394959996E-2</v>
       </c>
       <c r="V10" s="2">
         <f>ABS(S10)/$H10</f>
-        <v>6.195608822916087E-2</v>
+        <v>6.6177315394959996E-2</v>
       </c>
       <c r="W10" s="2">
         <f>ABS(T10)/$H10</f>
+        <v>6.195608822916087E-2</v>
+      </c>
+      <c r="X10" s="2">
+        <f>ABS(U10)/$H10</f>
         <v>4.2212271657991211E-3</v>
       </c>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-    </row>
-    <row r="11" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y10" s="2">
+        <f t="shared" si="16"/>
+        <v>0.13235463078991999</v>
+      </c>
+      <c r="Z10" s="2"/>
+    </row>
+    <row r="11" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>13</v>
       </c>
@@ -1325,66 +1389,73 @@
         <v>1.7521686195965265</v>
       </c>
       <c r="I11" s="2">
-        <f>E11-D11</f>
+        <f t="shared" si="0"/>
         <v>2.7721766388911053</v>
       </c>
       <c r="J11" s="2">
-        <f>F11-D11</f>
+        <f t="shared" si="1"/>
         <v>2.8182700049844716</v>
       </c>
       <c r="K11" s="2">
-        <f>F11-E11</f>
+        <f t="shared" si="2"/>
         <v>4.6093366093366228E-2</v>
       </c>
       <c r="L11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.5821403304948225</v>
       </c>
       <c r="M11" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.6084467975653149</v>
       </c>
       <c r="N11" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.6306467070492445E-2</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11" s="10">
+        <f t="shared" si="9"/>
+        <v>3.2168935951306299</v>
+      </c>
+      <c r="P11" s="2">
         <v>3.7216981132075473</v>
       </c>
-      <c r="P11" s="2">
+      <c r="Q11" s="2">
         <v>5.0424528301886795</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="R11" s="2">
         <v>5.4339622641509431</v>
       </c>
-      <c r="R11" s="2">
-        <f t="shared" si="6"/>
+      <c r="S11" s="2">
+        <f t="shared" si="10"/>
         <v>1.3207547169811322</v>
       </c>
-      <c r="S11" s="2">
-        <f t="shared" si="7"/>
+      <c r="T11" s="2">
+        <f t="shared" si="11"/>
         <v>1.7122641509433958</v>
       </c>
-      <c r="T11" s="2">
-        <f t="shared" si="8"/>
+      <c r="U11" s="2">
+        <f t="shared" si="12"/>
         <v>0.39150943396226356</v>
       </c>
-      <c r="U11" s="2">
-        <f t="shared" si="9"/>
+      <c r="V11" s="2">
+        <f t="shared" si="13"/>
         <v>0.75378288494018553</v>
       </c>
-      <c r="V11" s="2">
-        <f t="shared" si="10"/>
+      <c r="W11" s="2">
+        <f t="shared" si="14"/>
         <v>0.97722566869031158</v>
       </c>
-      <c r="W11" s="9">
-        <f t="shared" si="11"/>
+      <c r="X11" s="9">
+        <f t="shared" si="15"/>
         <v>0.22344278375012608</v>
       </c>
-      <c r="X11" s="10"/>
-      <c r="Y11" s="2"/>
-    </row>
-    <row r="12" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y11" s="10">
+        <f t="shared" si="16"/>
+        <v>1.9544513373806232</v>
+      </c>
+      <c r="Z11" s="2"/>
+    </row>
+    <row r="12" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>16</v>
       </c>
@@ -1404,66 +1475,73 @@
         <v>98496.685620379765</v>
       </c>
       <c r="I12" s="6">
-        <f>E12-D12</f>
+        <f t="shared" si="0"/>
         <v>205688.65915131854</v>
       </c>
       <c r="J12" s="6">
-        <f>F12-D12</f>
+        <f t="shared" si="1"/>
         <v>153435.12706531171</v>
       </c>
       <c r="K12" s="6">
-        <f>F12-E12</f>
+        <f t="shared" si="2"/>
         <v>-52253.53208600686</v>
       </c>
       <c r="L12" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.0882800051168409</v>
       </c>
       <c r="M12" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1.5577694426863511</v>
       </c>
       <c r="N12" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.53051056243049033</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12" s="10">
+        <f t="shared" si="9"/>
+        <v>4.1765600102336826</v>
+      </c>
+      <c r="P12" s="3">
         <v>88462.7706263281</v>
       </c>
-      <c r="P12" s="3">
+      <c r="Q12" s="3">
         <v>152470.82028311311</v>
       </c>
-      <c r="Q12" s="3">
+      <c r="R12" s="3">
         <v>179691.74007889573</v>
       </c>
-      <c r="R12" s="6">
-        <f t="shared" si="6"/>
+      <c r="S12" s="6">
+        <f t="shared" si="10"/>
         <v>64008.049656785006</v>
       </c>
-      <c r="S12" s="6">
-        <f t="shared" si="7"/>
+      <c r="T12" s="6">
+        <f t="shared" si="11"/>
         <v>91228.969452567631</v>
       </c>
-      <c r="T12" s="6">
-        <f t="shared" si="8"/>
+      <c r="U12" s="6">
+        <f t="shared" si="12"/>
         <v>27220.919795782625</v>
       </c>
-      <c r="U12" s="2">
-        <f t="shared" si="9"/>
+      <c r="V12" s="2">
+        <f t="shared" si="13"/>
         <v>0.64984978178332953</v>
       </c>
-      <c r="V12" s="2">
-        <f t="shared" si="10"/>
+      <c r="W12" s="2">
+        <f t="shared" si="14"/>
         <v>0.92621359671103098</v>
       </c>
-      <c r="W12" s="9">
-        <f t="shared" si="11"/>
+      <c r="X12" s="9">
+        <f t="shared" si="15"/>
         <v>0.27636381492770146</v>
       </c>
-      <c r="X12" s="2"/>
-      <c r="Y12" s="2"/>
-    </row>
-    <row r="13" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y12" s="10">
+        <f t="shared" si="16"/>
+        <v>1.852427193422062</v>
+      </c>
+      <c r="Z12" s="2"/>
+    </row>
+    <row r="13" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>17</v>
       </c>
@@ -1483,66 +1561,73 @@
         <v>0.23303067456676291</v>
       </c>
       <c r="I13" s="2">
-        <f>E13-D13</f>
+        <f t="shared" si="0"/>
         <v>2.2029731615012871E-2</v>
       </c>
       <c r="J13" s="2">
-        <f>F13-D13</f>
+        <f t="shared" si="1"/>
         <v>2.1847381904644303E-2</v>
       </c>
       <c r="K13" s="2">
-        <f>F13-E13</f>
+        <f t="shared" si="2"/>
         <v>-1.8234971036856784E-4</v>
       </c>
       <c r="L13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>9.4535758676274131E-2</v>
       </c>
       <c r="M13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>9.3753244911905634E-2</v>
       </c>
       <c r="N13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>7.8251376436849708E-4</v>
       </c>
       <c r="O13" s="2">
+        <f t="shared" si="9"/>
+        <v>0.18907151735254826</v>
+      </c>
+      <c r="P13" s="2">
         <v>0.83468288916981115</v>
       </c>
-      <c r="P13" s="2">
+      <c r="Q13" s="2">
         <v>0.81101564838679263</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="R13" s="2">
         <v>0.8131971603632081</v>
       </c>
-      <c r="R13" s="2">
-        <f t="shared" si="6"/>
+      <c r="S13" s="2">
+        <f t="shared" si="10"/>
         <v>-2.3667240783018517E-2</v>
       </c>
-      <c r="S13" s="2">
-        <f t="shared" si="7"/>
+      <c r="T13" s="2">
+        <f t="shared" si="11"/>
         <v>-2.1485728806603044E-2</v>
       </c>
-      <c r="T13" s="2">
-        <f t="shared" si="8"/>
+      <c r="U13" s="2">
+        <f t="shared" si="12"/>
         <v>2.1815119764154733E-3</v>
       </c>
-      <c r="U13" s="2">
-        <f t="shared" si="9"/>
+      <c r="V13" s="2">
+        <f t="shared" si="13"/>
         <v>0.10156276991009563</v>
       </c>
-      <c r="V13" s="2">
-        <f t="shared" si="10"/>
+      <c r="W13" s="2">
+        <f t="shared" si="14"/>
         <v>9.2201290008485204E-2</v>
       </c>
-      <c r="W13" s="2">
-        <f t="shared" si="11"/>
+      <c r="X13" s="2">
+        <f t="shared" si="15"/>
         <v>9.3614799016104363E-3</v>
       </c>
-      <c r="X13" s="2"/>
-      <c r="Y13" s="2"/>
-    </row>
-    <row r="14" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y13" s="2">
+        <f t="shared" si="16"/>
+        <v>0.20312553982019127</v>
+      </c>
+      <c r="Z13" s="2"/>
+    </row>
+    <row r="14" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>18</v>
       </c>
@@ -1562,66 +1647,73 @@
         <v>9.4934043771748439E-2</v>
       </c>
       <c r="I14" s="2">
-        <f>E14-D14</f>
+        <f t="shared" si="0"/>
         <v>-1.9105587015499768E-2</v>
       </c>
       <c r="J14" s="2">
-        <f>F14-D14</f>
+        <f t="shared" si="1"/>
         <v>-1.4014707806408858E-2</v>
       </c>
       <c r="K14" s="2">
-        <f>F14-E14</f>
+        <f t="shared" si="2"/>
         <v>5.0908792090909099E-3</v>
       </c>
       <c r="L14" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.20125116614052238</v>
       </c>
       <c r="M14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.14762573308374666</v>
       </c>
       <c r="N14" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>5.3625433056775702E-2</v>
       </c>
       <c r="O14" s="2">
+        <f t="shared" si="9"/>
+        <v>0.40250233228104471</v>
+      </c>
+      <c r="P14" s="2">
         <v>1.345688404245283E-2</v>
       </c>
-      <c r="P14" s="2">
+      <c r="Q14" s="2">
         <v>0</v>
       </c>
-      <c r="Q14" s="2">
+      <c r="R14" s="2">
         <v>5.2829878584905671E-3</v>
       </c>
-      <c r="R14" s="2">
-        <f t="shared" si="6"/>
+      <c r="S14" s="2">
+        <f t="shared" si="10"/>
         <v>-1.345688404245283E-2</v>
       </c>
-      <c r="S14" s="2">
-        <f t="shared" si="7"/>
+      <c r="T14" s="2">
+        <f t="shared" si="11"/>
         <v>-8.173896183962262E-3</v>
       </c>
-      <c r="T14" s="2">
-        <f t="shared" si="8"/>
+      <c r="U14" s="2">
+        <f t="shared" si="12"/>
         <v>5.2829878584905671E-3</v>
       </c>
-      <c r="U14" s="2">
-        <f t="shared" si="9"/>
+      <c r="V14" s="2">
+        <f t="shared" si="13"/>
         <v>0.14174982448664517</v>
       </c>
-      <c r="V14" s="2">
-        <f t="shared" si="10"/>
+      <c r="W14" s="2">
+        <f t="shared" si="14"/>
         <v>8.6100790182443945E-2</v>
       </c>
-      <c r="W14" s="2">
-        <f t="shared" si="11"/>
+      <c r="X14" s="2">
+        <f t="shared" si="15"/>
         <v>5.5649034304201199E-2</v>
       </c>
-      <c r="X14" s="2"/>
-      <c r="Y14" s="2"/>
-    </row>
-    <row r="15" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y14" s="2">
+        <f t="shared" si="16"/>
+        <v>0.28349964897329033</v>
+      </c>
+      <c r="Z14" s="2"/>
+    </row>
+    <row r="15" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>19</v>
       </c>
@@ -1641,66 +1733,73 @@
         <v>996.37465552063486</v>
       </c>
       <c r="I15" s="2">
-        <f>E15-D15</f>
+        <f t="shared" si="0"/>
         <v>-40.90523485950731</v>
       </c>
       <c r="J15" s="2">
-        <f>F15-D15</f>
+        <f t="shared" si="1"/>
         <v>2691.8979769832436</v>
       </c>
       <c r="K15" s="2">
-        <f>F15-E15</f>
+        <f t="shared" si="2"/>
         <v>2732.8032118427509</v>
       </c>
       <c r="L15" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4.1054070005557428E-2</v>
       </c>
       <c r="M15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2.7016925431294196</v>
       </c>
       <c r="N15" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.7427466131349774</v>
       </c>
-      <c r="O15" s="2">
+      <c r="O15" s="10">
+        <f t="shared" si="9"/>
+        <v>5.4854932262699538</v>
+      </c>
+      <c r="P15" s="2">
         <v>1.0168066981132075E-4</v>
       </c>
-      <c r="P15" s="2">
+      <c r="Q15" s="2">
         <v>9.3406485849056617E-5</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="R15" s="2">
         <v>2.8215410283018868E-3</v>
       </c>
-      <c r="R15" s="2">
-        <f t="shared" si="6"/>
+      <c r="S15" s="2">
+        <f t="shared" si="10"/>
         <v>-8.2741839622641324E-6</v>
       </c>
-      <c r="S15" s="2">
-        <f t="shared" si="7"/>
+      <c r="T15" s="2">
+        <f t="shared" si="11"/>
         <v>2.719860358490566E-3</v>
       </c>
-      <c r="T15" s="2">
-        <f t="shared" si="8"/>
+      <c r="U15" s="2">
+        <f t="shared" si="12"/>
         <v>2.7281345424528302E-3</v>
       </c>
-      <c r="U15" s="2">
-        <f t="shared" si="9"/>
+      <c r="V15" s="2">
+        <f t="shared" si="13"/>
         <v>8.3042898737128445E-9</v>
       </c>
-      <c r="V15" s="9">
-        <f t="shared" si="10"/>
+      <c r="W15" s="9">
+        <f t="shared" si="14"/>
         <v>2.729756666752387E-6</v>
       </c>
-      <c r="W15" s="2">
-        <f t="shared" si="11"/>
+      <c r="X15" s="2">
+        <f t="shared" si="15"/>
         <v>2.7380609566261E-6</v>
       </c>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="2"/>
-    </row>
-    <row r="16" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y15" s="2">
+        <f t="shared" si="16"/>
+        <v>5.4761219132522E-6</v>
+      </c>
+      <c r="Z15" s="2"/>
+    </row>
+    <row r="16" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>30</v>
       </c>
@@ -1720,66 +1819,73 @@
         <v>3.9759102838589626E-2</v>
       </c>
       <c r="I16" s="7">
-        <f>E16-D16</f>
+        <f t="shared" si="0"/>
         <v>2.1126043107258519E-2</v>
       </c>
       <c r="J16" s="7">
-        <f>F16-D16</f>
+        <f t="shared" si="1"/>
         <v>7.0889715103928941E-3</v>
       </c>
       <c r="K16" s="7">
-        <f>F16-E16</f>
+        <f t="shared" si="2"/>
         <v>-1.4037071596865625E-2</v>
       </c>
       <c r="L16" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.53135110198598035</v>
       </c>
       <c r="M16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.17829807526523053</v>
       </c>
       <c r="N16" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.35305302672074984</v>
       </c>
       <c r="O16" s="2">
+        <f t="shared" si="9"/>
+        <v>1.0627022039719607</v>
+      </c>
+      <c r="P16" s="2">
         <v>0.58190653180188678</v>
       </c>
-      <c r="P16" s="2">
+      <c r="Q16" s="2">
         <v>0.57688346348113229</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="R16" s="2">
         <v>0.57025366976886827</v>
       </c>
-      <c r="R16" s="7">
-        <f t="shared" si="6"/>
+      <c r="S16" s="7">
+        <f t="shared" si="10"/>
         <v>-5.0230683207544979E-3</v>
       </c>
-      <c r="S16" s="7">
-        <f t="shared" si="7"/>
+      <c r="T16" s="7">
+        <f t="shared" si="11"/>
         <v>-1.1652862033018518E-2</v>
       </c>
-      <c r="T16" s="7">
-        <f t="shared" si="8"/>
+      <c r="U16" s="7">
+        <f t="shared" si="12"/>
         <v>-6.6297937122640205E-3</v>
       </c>
-      <c r="U16" s="2">
-        <f t="shared" si="9"/>
+      <c r="V16" s="2">
+        <f t="shared" si="13"/>
         <v>0.1263375670509139</v>
       </c>
-      <c r="V16" s="2">
-        <f t="shared" si="10"/>
+      <c r="W16" s="2">
+        <f t="shared" si="14"/>
         <v>0.29308664434219611</v>
       </c>
-      <c r="W16" s="2">
-        <f t="shared" si="11"/>
+      <c r="X16" s="2">
+        <f t="shared" si="15"/>
         <v>0.16674907729128224</v>
       </c>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="2"/>
-    </row>
-    <row r="17" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y16" s="2">
+        <f t="shared" si="16"/>
+        <v>0.58617328868439222</v>
+      </c>
+      <c r="Z16" s="2"/>
+    </row>
+    <row r="17" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>20</v>
       </c>
@@ -1799,66 +1905,73 @@
         <v>197.14430648420787</v>
       </c>
       <c r="I17" s="7">
-        <f>E17-D17</f>
+        <f t="shared" si="0"/>
         <v>180.19479476101998</v>
       </c>
       <c r="J17" s="7">
-        <f>F17-D17</f>
+        <f t="shared" si="1"/>
         <v>79.355335301560501</v>
       </c>
       <c r="K17" s="7">
-        <f>F17-E17</f>
+        <f t="shared" si="2"/>
         <v>-100.83945945945948</v>
       </c>
       <c r="L17" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.91402484796310546</v>
       </c>
       <c r="M17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.40252410387472798</v>
       </c>
       <c r="N17" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.51150074408837753</v>
       </c>
-      <c r="O17" s="4">
+      <c r="O17" s="2">
+        <f t="shared" si="9"/>
+        <v>1.8280496959262109</v>
+      </c>
+      <c r="P17" s="4">
         <v>488.20754716981133</v>
       </c>
-      <c r="P17" s="4">
+      <c r="Q17" s="4">
         <v>502.36320754716979</v>
       </c>
-      <c r="Q17" s="4">
+      <c r="R17" s="4">
         <v>492.68867924528303</v>
       </c>
-      <c r="R17" s="4">
-        <f t="shared" si="6"/>
+      <c r="S17" s="4">
+        <f t="shared" si="10"/>
         <v>14.155660377358458</v>
       </c>
-      <c r="S17" s="4">
-        <f t="shared" si="7"/>
+      <c r="T17" s="4">
+        <f t="shared" si="11"/>
         <v>4.4811320754716917</v>
       </c>
-      <c r="T17" s="4">
-        <f t="shared" si="8"/>
+      <c r="U17" s="4">
+        <f t="shared" si="12"/>
         <v>-9.6745283018867667</v>
       </c>
-      <c r="U17" s="2">
-        <f t="shared" si="9"/>
+      <c r="V17" s="2">
+        <f t="shared" si="13"/>
         <v>7.1803546497511403E-2</v>
       </c>
-      <c r="V17" s="2">
-        <f t="shared" si="10"/>
+      <c r="W17" s="2">
+        <f t="shared" si="14"/>
         <v>2.2730212986549779E-2</v>
       </c>
-      <c r="W17" s="2">
-        <f t="shared" si="11"/>
+      <c r="X17" s="2">
+        <f t="shared" si="15"/>
         <v>4.9073333510961624E-2</v>
       </c>
-      <c r="X17" s="7"/>
-      <c r="Y17" s="2"/>
-    </row>
-    <row r="18" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y17" s="2">
+        <f t="shared" si="16"/>
+        <v>0.14360709299502281</v>
+      </c>
+      <c r="Z17" s="2"/>
+    </row>
+    <row r="18" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>31</v>
       </c>
@@ -1878,15 +1991,15 @@
         <v>0.34195074381377394</v>
       </c>
       <c r="I18" s="7">
-        <f>E18-D18</f>
+        <f t="shared" si="0"/>
         <v>-0.35787134485020289</v>
       </c>
       <c r="J18" s="7">
-        <f>F18-D18</f>
+        <f t="shared" si="1"/>
         <v>-0.19972660494314365</v>
       </c>
       <c r="K18" s="7">
-        <f>F18-E18</f>
+        <f t="shared" si="2"/>
         <v>0.15814473990705924</v>
       </c>
       <c r="L18" s="7">
@@ -1901,43 +2014,50 @@
         <f>ABS(K18)/$H18</f>
         <v>0.46247812811655914</v>
       </c>
-      <c r="O18" s="2">
+      <c r="O18" s="10">
+        <f t="shared" si="9"/>
+        <v>2.093116341019567</v>
+      </c>
+      <c r="P18" s="2">
         <v>2.7140556088584895</v>
       </c>
-      <c r="P18" s="2">
+      <c r="Q18" s="2">
         <v>2.6671574119339616</v>
       </c>
-      <c r="Q18" s="2">
+      <c r="R18" s="2">
         <v>2.6213917499198116</v>
       </c>
-      <c r="R18" s="7">
-        <f>P18-O18</f>
+      <c r="S18" s="7">
+        <f>Q18-P18</f>
         <v>-4.6898196924527902E-2</v>
       </c>
-      <c r="S18" s="7">
-        <f>Q18-O18</f>
+      <c r="T18" s="7">
+        <f>R18-P18</f>
         <v>-9.2663858938677901E-2</v>
       </c>
-      <c r="T18" s="7">
-        <f>Q18-P18</f>
+      <c r="U18" s="7">
+        <f>R18-Q18</f>
         <v>-4.5765662014149999E-2</v>
-      </c>
-      <c r="U18" s="2">
-        <f>ABS(R18)/$H18</f>
-        <v>0.13714898350994265</v>
       </c>
       <c r="V18" s="2">
         <f>ABS(S18)/$H18</f>
-        <v>0.27098598442921518</v>
+        <v>0.13714898350994265</v>
       </c>
       <c r="W18" s="2">
         <f>ABS(T18)/$H18</f>
+        <v>0.27098598442921518</v>
+      </c>
+      <c r="X18" s="2">
+        <f>ABS(U18)/$H18</f>
         <v>0.13383700091927256</v>
       </c>
-      <c r="X18" s="7"/>
-      <c r="Y18" s="2"/>
-    </row>
-    <row r="19" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y18" s="2">
+        <f t="shared" si="16"/>
+        <v>0.54197196885843035</v>
+      </c>
+      <c r="Z18" s="2"/>
+    </row>
+    <row r="19" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
         <v>21</v>
       </c>
@@ -1957,66 +2077,73 @@
         <v>2.2329600236650895E-2</v>
       </c>
       <c r="I19" s="7">
-        <f>E19-D19</f>
+        <f t="shared" si="0"/>
         <v>9.4244072785919855E-3</v>
       </c>
       <c r="J19" s="7">
-        <f>F19-D19</f>
+        <f t="shared" si="1"/>
         <v>2.2999970862332478E-3</v>
       </c>
       <c r="K19" s="7">
-        <f>F19-E19</f>
+        <f t="shared" si="2"/>
         <v>-7.1244101923587377E-3</v>
       </c>
       <c r="L19" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.42205893427161084</v>
       </c>
       <c r="M19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.10300216134000136</v>
       </c>
       <c r="N19" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.3190567729316095</v>
       </c>
       <c r="O19" s="2">
+        <f t="shared" si="9"/>
+        <v>0.84411786854322168</v>
+      </c>
+      <c r="P19" s="2">
         <v>3.9798378754716986E-2</v>
       </c>
-      <c r="P19" s="2">
+      <c r="Q19" s="2">
         <v>3.735397834905662E-2</v>
       </c>
-      <c r="Q19" s="2">
+      <c r="R19" s="2">
         <v>3.7867497042452819E-2</v>
       </c>
-      <c r="R19" s="7">
-        <f t="shared" si="6"/>
+      <c r="S19" s="7">
+        <f t="shared" si="10"/>
         <v>-2.4444004056603658E-3</v>
       </c>
-      <c r="S19" s="7">
-        <f t="shared" si="7"/>
+      <c r="T19" s="7">
+        <f t="shared" si="11"/>
         <v>-1.9308817122641667E-3</v>
       </c>
-      <c r="T19" s="7">
-        <f t="shared" si="8"/>
+      <c r="U19" s="7">
+        <f t="shared" si="12"/>
         <v>5.135186933961991E-4</v>
       </c>
-      <c r="U19" s="2">
-        <f t="shared" si="9"/>
+      <c r="V19" s="2">
+        <f t="shared" si="13"/>
         <v>0.10946906257856899</v>
       </c>
-      <c r="V19" s="2">
-        <f t="shared" si="10"/>
+      <c r="W19" s="2">
+        <f t="shared" si="14"/>
         <v>8.6471844179946231E-2</v>
       </c>
-      <c r="W19" s="2">
-        <f t="shared" si="11"/>
+      <c r="X19" s="2">
+        <f t="shared" si="15"/>
         <v>2.299721839862276E-2</v>
       </c>
-      <c r="X19" s="7"/>
-      <c r="Y19" s="2"/>
-    </row>
-    <row r="20" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y19" s="2">
+        <f t="shared" si="16"/>
+        <v>0.21893812515713798</v>
+      </c>
+      <c r="Z19" s="2"/>
+    </row>
+    <row r="20" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>22</v>
       </c>
@@ -2036,66 +2163,73 @@
         <v>0.15410945985308402</v>
       </c>
       <c r="I20" s="7">
-        <f>E20-D20</f>
+        <f t="shared" si="0"/>
         <v>0.20324039601040106</v>
       </c>
       <c r="J20" s="7">
-        <f>F20-D20</f>
+        <f t="shared" si="1"/>
         <v>9.2685942113079622E-2</v>
       </c>
       <c r="K20" s="7">
-        <f>F20-E20</f>
+        <f t="shared" si="2"/>
         <v>-0.11055445389732144</v>
       </c>
       <c r="L20" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.3188054529822806</v>
       </c>
       <c r="M20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.60142928410390373</v>
       </c>
       <c r="N20" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.71737616887837685</v>
       </c>
-      <c r="O20" s="2">
+      <c r="O20" s="10">
+        <f t="shared" si="9"/>
+        <v>2.6376109059645612</v>
+      </c>
+      <c r="P20" s="2">
         <v>0.49196611640566046</v>
       </c>
-      <c r="P20" s="2">
+      <c r="Q20" s="2">
         <v>0.58236738790094367</v>
       </c>
-      <c r="Q20" s="2">
+      <c r="R20" s="2">
         <v>0.50184743726415093</v>
       </c>
-      <c r="R20" s="7">
-        <f t="shared" si="6"/>
+      <c r="S20" s="7">
+        <f t="shared" si="10"/>
         <v>9.0401271495283209E-2</v>
       </c>
-      <c r="S20" s="7">
-        <f t="shared" si="7"/>
+      <c r="T20" s="7">
+        <f t="shared" si="11"/>
         <v>9.8813208584904721E-3</v>
       </c>
-      <c r="T20" s="7">
-        <f t="shared" si="8"/>
+      <c r="U20" s="7">
+        <f t="shared" si="12"/>
         <v>-8.0519950636792736E-2</v>
       </c>
-      <c r="U20" s="2">
-        <f t="shared" si="9"/>
+      <c r="V20" s="2">
+        <f t="shared" si="13"/>
         <v>0.58660429788972557</v>
       </c>
-      <c r="V20" s="2">
-        <f t="shared" si="10"/>
+      <c r="W20" s="2">
+        <f t="shared" si="14"/>
         <v>6.4118846876178498E-2</v>
       </c>
-      <c r="W20" s="2">
-        <f t="shared" si="11"/>
+      <c r="X20" s="2">
+        <f t="shared" si="15"/>
         <v>0.52248545101354715</v>
       </c>
-      <c r="X20" s="7"/>
-      <c r="Y20" s="2"/>
-    </row>
-    <row r="21" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y20" s="10">
+        <f t="shared" si="16"/>
+        <v>1.1732085957794514</v>
+      </c>
+      <c r="Z20" s="2"/>
+    </row>
+    <row r="21" spans="3:26" x14ac:dyDescent="0.35">
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="13"/>
@@ -2106,19 +2240,26 @@
       <c r="L21" s="7"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
+      <c r="O21" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
-      <c r="R21" s="7"/>
+      <c r="R21" s="2"/>
       <c r="S21" s="7"/>
       <c r="T21" s="7"/>
-      <c r="U21" s="2"/>
+      <c r="U21" s="7"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
-      <c r="X21" s="7"/>
-      <c r="Y21" s="2"/>
-    </row>
-    <row r="22" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="Z21" s="2"/>
+    </row>
+    <row r="22" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C22" s="11" t="s">
         <v>10</v>
       </c>
@@ -2150,54 +2291,61 @@
         <v>3.3764158255082943E-2</v>
       </c>
       <c r="L22" s="2">
-        <f t="shared" ref="L22:N24" si="21">ABS(I22)/$H22</f>
+        <f t="shared" ref="L22:N24" si="26">ABS(I22)/$H22</f>
         <v>0.68731972988520806</v>
       </c>
       <c r="M22" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.88437094567756525</v>
       </c>
       <c r="N22" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.19705121579235715</v>
       </c>
       <c r="O22" s="2">
+        <f t="shared" si="9"/>
+        <v>1.7687418913551305</v>
+      </c>
+      <c r="P22" s="2">
         <v>0.36450349562112333</v>
       </c>
-      <c r="P22" s="2">
+      <c r="Q22" s="2">
         <v>0.42253427072203753</v>
       </c>
-      <c r="Q22" s="2">
+      <c r="R22" s="2">
         <v>0.4691327597068693</v>
       </c>
-      <c r="R22" s="2">
-        <f>P22-O22</f>
+      <c r="S22" s="2">
+        <f>Q22-P22</f>
         <v>5.80307751009142E-2</v>
       </c>
-      <c r="S22" s="2">
-        <f>Q22-O22</f>
+      <c r="T22" s="2">
+        <f>R22-P22</f>
         <v>0.10462926408574597</v>
       </c>
-      <c r="T22" s="2">
-        <f>Q22-P22</f>
+      <c r="U22" s="2">
+        <f>R22-Q22</f>
         <v>4.6598488984831765E-2</v>
       </c>
-      <c r="U22" s="2">
-        <f t="shared" ref="U22:W24" si="22">ABS(R22)/$H22</f>
+      <c r="V22" s="2">
+        <f t="shared" ref="V22:X24" si="27">ABS(S22)/$H22</f>
         <v>0.338673770588862</v>
       </c>
-      <c r="V22" s="2">
-        <f t="shared" si="22"/>
+      <c r="W22" s="2">
+        <f t="shared" si="27"/>
         <v>0.61062750446183767</v>
       </c>
-      <c r="W22" s="2">
-        <f t="shared" si="22"/>
+      <c r="X22" s="2">
+        <f t="shared" si="27"/>
         <v>0.27195373387297572</v>
       </c>
-      <c r="X22" s="2"/>
-      <c r="Y22" s="2"/>
-    </row>
-    <row r="23" spans="3:25" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y22" s="10">
+        <f t="shared" si="16"/>
+        <v>1.2212550089236753</v>
+      </c>
+      <c r="Z22" s="2"/>
+    </row>
+    <row r="23" spans="3:26" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C23" s="11" t="s">
         <v>12</v>
       </c>
@@ -2229,54 +2377,61 @@
         <v>0.32965601965601971</v>
       </c>
       <c r="L23" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>4.7234391729800554E-2</v>
       </c>
       <c r="M23" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>2.765966644787055</v>
       </c>
       <c r="N23" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>2.8132010365168556</v>
       </c>
-      <c r="O23" s="2">
+      <c r="O23" s="10">
+        <f t="shared" si="9"/>
+        <v>5.6264020730337112</v>
+      </c>
+      <c r="P23" s="2">
         <v>1.4150943396226415E-2</v>
       </c>
-      <c r="P23" s="2">
+      <c r="Q23" s="2">
         <v>0</v>
       </c>
-      <c r="Q23" s="2">
+      <c r="R23" s="2">
         <v>0.330188679245283</v>
       </c>
-      <c r="R23" s="2">
-        <f>P23-O23</f>
+      <c r="S23" s="2">
+        <f>Q23-P23</f>
         <v>-1.4150943396226415E-2</v>
       </c>
-      <c r="S23" s="2">
-        <f>Q23-O23</f>
+      <c r="T23" s="2">
+        <f>R23-P23</f>
         <v>0.31603773584905659</v>
       </c>
-      <c r="T23" s="2">
-        <f>Q23-P23</f>
+      <c r="U23" s="2">
+        <f>R23-Q23</f>
         <v>0.330188679245283</v>
       </c>
-      <c r="U23" s="2">
-        <f t="shared" si="22"/>
+      <c r="V23" s="2">
+        <f t="shared" si="27"/>
         <v>0.12076056937014153</v>
       </c>
-      <c r="V23" s="2">
-        <f t="shared" si="22"/>
+      <c r="W23" s="2">
+        <f t="shared" si="27"/>
         <v>2.6969860492664939</v>
       </c>
-      <c r="W23" s="9">
-        <f t="shared" si="22"/>
+      <c r="X23" s="9">
+        <f t="shared" si="27"/>
         <v>2.8177466186366353</v>
       </c>
-      <c r="X23" s="2"/>
-      <c r="Y23" s="2"/>
-    </row>
-    <row r="24" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y23" s="10">
+        <f t="shared" si="16"/>
+        <v>5.6354932372732707</v>
+      </c>
+      <c r="Z23" s="2"/>
+    </row>
+    <row r="24" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C24" s="11" t="s">
         <v>15</v>
       </c>
@@ -2308,54 +2463,61 @@
         <v>9.8968058968058964E-2</v>
       </c>
       <c r="L24" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.88169960560275762</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>1.2945214361817865</v>
       </c>
       <c r="N24" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.41282183057902894</v>
       </c>
-      <c r="O24" s="2">
+      <c r="O24" s="10">
+        <f t="shared" si="9"/>
+        <v>2.589042872363573</v>
+      </c>
+      <c r="P24" s="2">
         <v>8.0188679245283015E-2</v>
       </c>
-      <c r="P24" s="2">
+      <c r="Q24" s="2">
         <v>0.17452830188679244</v>
       </c>
-      <c r="Q24" s="2">
+      <c r="R24" s="2">
         <v>0.35377358490566035</v>
       </c>
-      <c r="R24" s="2">
-        <f>P24-O24</f>
+      <c r="S24" s="2">
+        <f>Q24-P24</f>
         <v>9.4339622641509427E-2</v>
       </c>
-      <c r="S24" s="2">
-        <f>Q24-O24</f>
+      <c r="T24" s="2">
+        <f>R24-P24</f>
         <v>0.27358490566037735</v>
       </c>
-      <c r="T24" s="2">
-        <f>Q24-P24</f>
+      <c r="U24" s="2">
+        <f>R24-Q24</f>
         <v>0.17924528301886791</v>
       </c>
-      <c r="U24" s="2">
-        <f t="shared" si="22"/>
+      <c r="V24" s="2">
+        <f t="shared" si="27"/>
         <v>0.3935154040716512</v>
       </c>
-      <c r="V24" s="2">
-        <f t="shared" si="22"/>
+      <c r="W24" s="2">
+        <f t="shared" si="27"/>
         <v>1.1411946718077886</v>
       </c>
-      <c r="W24" s="9">
-        <f t="shared" si="22"/>
+      <c r="X24" s="9">
+        <f t="shared" si="27"/>
         <v>0.74767926773613724</v>
       </c>
-      <c r="X24" s="2"/>
-      <c r="Y24" s="2"/>
-    </row>
-    <row r="25" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="Y24" s="10">
+        <f t="shared" si="16"/>
+        <v>2.2823893436155771</v>
+      </c>
+      <c r="Z24" s="2"/>
+    </row>
+    <row r="25" spans="3:26" x14ac:dyDescent="0.35">
       <c r="L25" s="8">
         <f>COUNTIF(L4:L24,"&lt;0.25")</f>
         <v>4</v>
@@ -2368,60 +2530,57 @@
         <f>COUNTIF(N4:N24,"&lt;0.25")</f>
         <v>5</v>
       </c>
-      <c r="T25" t="s">
+      <c r="O25" s="2"/>
+      <c r="U25" t="s">
         <v>33</v>
-      </c>
-      <c r="U25" s="8">
-        <f>COUNTIF(U4:U24,"&lt;0.25")</f>
-        <v>13</v>
       </c>
       <c r="V25" s="8">
         <f>COUNTIF(V4:V24,"&lt;0.25")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="W25" s="8">
         <f>COUNTIF(W4:W24,"&lt;0.25")</f>
+        <v>12</v>
+      </c>
+      <c r="X25" s="8">
+        <f>COUNTIF(X4:X24,"&lt;0.25")</f>
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="3:25" x14ac:dyDescent="0.35">
-      <c r="T26" t="s">
+    <row r="26" spans="3:26" x14ac:dyDescent="0.35">
+      <c r="U26" t="s">
         <v>32</v>
       </c>
-      <c r="U26" s="8">
-        <f>U25-L25</f>
+      <c r="V26" s="8">
+        <f>V25-L25</f>
         <v>9</v>
       </c>
-      <c r="V26" s="8">
-        <f t="shared" ref="V26:W26" si="23">V25-M25</f>
+      <c r="W26" s="8">
+        <f>W25-M25</f>
         <v>6</v>
       </c>
-      <c r="W26" s="8">
-        <f t="shared" si="23"/>
+      <c r="X26" s="8">
+        <f>X25-N25</f>
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="3:25" x14ac:dyDescent="0.35">
-      <c r="T27" t="s">
+    <row r="27" spans="3:26" x14ac:dyDescent="0.35">
+      <c r="U27" t="s">
         <v>34</v>
       </c>
-      <c r="U27">
+      <c r="V27">
         <v>0</v>
       </c>
-      <c r="V27">
+      <c r="W27">
         <v>1</v>
       </c>
-      <c r="W27">
+      <c r="X27">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="3:25" x14ac:dyDescent="0.35">
-      <c r="T28" t="s">
+    <row r="28" spans="3:26" x14ac:dyDescent="0.35">
+      <c r="U28" t="s">
         <v>35</v>
-      </c>
-      <c r="U28" s="8">
-        <f>COUNT(U4:U24)-U25-U27</f>
-        <v>7</v>
       </c>
       <c r="V28" s="8">
         <f>COUNT(V4:V24)-V25-V27</f>
@@ -2429,29 +2588,33 @@
       </c>
       <c r="W28" s="8">
         <f>COUNT(W4:W24)-W25-W27</f>
+        <v>7</v>
+      </c>
+      <c r="X28" s="8">
+        <f>COUNT(X4:X24)-X25-X27</f>
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="3:25" x14ac:dyDescent="0.35">
-      <c r="U29">
-        <f>U25+U27+U28</f>
+    <row r="29" spans="3:26" x14ac:dyDescent="0.35">
+      <c r="V29">
+        <f>V25+V27+V28</f>
         <v>20</v>
       </c>
-      <c r="V29">
-        <f t="shared" ref="V29:W29" si="24">V25+V27+V28</f>
+      <c r="W29">
+        <f t="shared" ref="W29:X29" si="28">W25+W27+W28</f>
         <v>20</v>
       </c>
-      <c r="W29">
-        <f t="shared" si="24"/>
+      <c r="X29">
+        <f t="shared" si="28"/>
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D1:K1"/>
-    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="P1:R1"/>
   </mergeCells>
-  <conditionalFormatting sqref="L4:N24 U4:W24">
+  <conditionalFormatting sqref="L4:O4 V4:X24 L5:N24 O5:O25">
     <cfRule type="cellIs" dxfId="4" priority="7" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
@@ -2461,17 +2624,17 @@
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U25:W25">
+  <conditionalFormatting sqref="V25:X25">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U26:W26">
+  <conditionalFormatting sqref="V26:X26">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U28:W28">
+  <conditionalFormatting sqref="V28:X28">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>

</xml_diff>